<commit_message>
feat: Mejoras en formulario SDR y exportación Excel
- Actualización de formulario SDR:
  - Labels fuera de campos de texto con hintText dentro
  - HintText en gris e itálica
  - Campos fijos: Grupo planificador (LD. 70), Puesto trabajo (PTAZ POZA RICA), Autor aviso (0117)
  - Dropdowns: Repercusión funcionamiento (3 opciones), Atención daño (3 opciones)
  - Sección 2: Campos fijos (Centro Emplazamiento, Puesto trabajo, División)
  - Dropdown Área de empresa (5 opciones)
  - Campo Emplazamiento fijo (PTAZ PORZA RICA)

- Exportación Excel:
  - Columna UBICACIÓN formateada como R{rack}-{contenedor}
  - Múltiples contenedores combinados en una celda separados por comas
  - Mejoras en búsqueda dinámica de columna UBICACIÓN

- Documentación:
  - Guía completa de despliegue para servicio Excel (GUIA_DESPLIEGUE_EXCEL.md)
</commit_message>
<xml_diff>
--- a/excel_generator_service/assets/templates/plantilla_jumpers.xlsx
+++ b/excel_generator_service/assets/templates/plantilla_jumpers.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Hoja 1'!$B$4:$F$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Hoja 1'!$B$4:$E$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">INVENTARIO JUMPERS </t>
   </si>
@@ -37,10 +37,7 @@
     <t xml:space="preserve">CANTIDAD</t>
   </si>
   <si>
-    <t xml:space="preserve">RACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#</t>
+    <t xml:space="preserve">UBICACIÓN</t>
   </si>
 </sst>
 </file>
@@ -102,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -125,13 +122,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -141,13 +131,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -178,7 +161,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,23 +186,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,18 +211,10 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -437,20 +404,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:L275"/>
+  <dimension ref="B1:K275"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -460,21 +429,18 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
@@ -489,1452 +455,1248 @@
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="7"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="7"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="7"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
+      <c r="F31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
-      <c r="F133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
-      <c r="F134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
-      <c r="F135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
-      <c r="F136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
-      <c r="F138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
-      <c r="F141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
-      <c r="F143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
-      <c r="F147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
-      <c r="F152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
-      <c r="F171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
-      <c r="F174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
-      <c r="F176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
-      <c r="F177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
-      <c r="F180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
-      <c r="F182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
-      <c r="F186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
-      <c r="F187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
-      <c r="F188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
-      <c r="F190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
-      <c r="F193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
-      <c r="F194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
-      <c r="F195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
-      <c r="F196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
-      <c r="F198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
-      <c r="F199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
-      <c r="F200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
-      <c r="F201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
-      <c r="F202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
-      <c r="F203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
-      <c r="F204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
-      <c r="F205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2007,9 +1769,9 @@
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="B4:F4"/>
+  <autoFilter ref="B4:E4"/>
   <mergeCells count="1">
-    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="B1:E2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>